<commit_message>
Integration robot for bank loan concolic
</commit_message>
<xml_diff>
--- a/TestingTool_Concolic/Applications/C#Models/SimpleBankLoanCSharp/ConfigurationFile/Config.xlsx
+++ b/TestingTool_Concolic/Applications/C#Models/SimpleBankLoanCSharp/ConfigurationFile/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubPhD\rpa-testing\TestingTool_v2\TestModels\ConfigurationFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GithubPhD\rpa-testing\TestingTool_Concolic\Applications\C#Models\SimpleBankLoanCSharp\ConfigurationFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F02140C-35AD-447B-A81E-943C99643002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9246C8CC-4AA5-4135-96C4-1F56C6182696}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="0" windowWidth="13824" windowHeight="7176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -75,13 +75,13 @@
     <t>testQueue</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingTool_v2</t>
+    <t>C:\GithubPhD\rpa-testing\TestingTool_Concolic</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingTool_v2\first.py</t>
+    <t>C:\GithubPhD\rpa-testing\TestingTool_Concolic\first.py</t>
   </si>
   <si>
-    <t>C:\GithubPhD\rpa-testing\TestingTool_v2\Applications\C#Models\SimpleBankLoanCSharp</t>
+    <t>C:\GithubPhD\rpa-testing\TestingTool_Concolic\Applications\C#Models\SimpleBankLoanCSharp</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>